<commit_message>
Sarah Daniel Task 09
</commit_message>
<xml_diff>
--- a/Project/data/TasDevil.xlsx
+++ b/Project/data/TasDevil.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahdaniel/Desktop/Evolution/Tasks/Task07/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahdaniel/Desktop/Evolution/Tasks/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="CaptureData" sheetId="1" r:id="rId1"/>
@@ -933,7 +933,7 @@
   <dimension ref="A1:J1978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>